<commit_message>
Added instructions on formatting
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Mercer\Google Drive\  QR\NC MAT 143\Videos\Tech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610DE188-97E1-435B-B2BB-FE3091B60E33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18315" windowHeight="10950"/>
+    <workbookView xWindow="1920" yWindow="1080" windowWidth="20796" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Original Amount</t>
   </si>
@@ -39,12 +40,15 @@
   </si>
   <si>
     <t>% Change (percent form)</t>
+  </si>
+  <si>
+    <t>Use formulas to calculate the Amount of Change, % Change (decimal form), and % Change (percent form) in cells C2, D2, E2, C3, D3, and E3.  Format the decimal form to four decima places and the "percent form" to two decimals.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -91,10 +95,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,101 +118,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1905000" y="762000"/>
-          <a:ext cx="4314825" cy="523875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Use</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> formulas to calculate the Amount of Change, % Change (decimal form), and % Change (percent form) in cells C2, D2, E2, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>C3, D3, and E3.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>  </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,23 +382,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3.5</v>
       </c>
@@ -514,7 +426,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6.55</v>
       </c>
@@ -525,8 +437,27 @@
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C5:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed video and link
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{4EE164FE-E69E-47B0-B5C1-E855FC58A498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{9EA94BE5-3165-4382-9DBC-71D092527226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="1470" windowWidth="17580" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,15 +247,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -724,6 +715,53 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,9 +788,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -780,7 +815,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -803,31 +843,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -852,14 +867,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -884,24 +891,8 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1094,8 +1085,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{43A8D30A-EEB9-4F2B-ADEB-F639691A7CDC}">
-  <header guid="{43A8D30A-EEB9-4F2B-ADEB-F639691A7CDC}" dateTime="2021-02-22T09:59:27" maxSheetId="4" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{88CE9DC2-ABFB-4BCA-BEFE-AAF543E2B318}">
+  <header guid="{88CE9DC2-ABFB-4BCA-BEFE-AAF543E2B318}" dateTime="2021-03-11T11:22:48" maxSheetId="4" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="3">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1111,7 +1102,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{43A8D30A-EEB9-4F2B-ADEB-F639691A7CDC}" name="Richard Ketchersid" id="-1739557268" dateTime="2021-02-22T09:59:27"/>
+  <userInfo guid="{88CE9DC2-ABFB-4BCA-BEFE-AAF543E2B318}" name="Richard Ketchersid" id="-1739579954" dateTime="2021-03-11T11:22:48"/>
 </users>
 </file>
 
@@ -1381,7 +1372,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1397,34 +1388,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="68" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1505,26 +1496,26 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
     </row>
     <row r="14" spans="1:8">
       <c r="D14" s="1" t="s">
@@ -1535,10 +1526,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1553,10 +1544,10 @@
       <c r="F16" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xMevCnl4KX/hTRbdGhqN2fdoBbT1naQOeJQ/7KVDNZUHBFLM7fALUHyllAA4Ygqw05A1AWSgYaboAyUmlHjRHQ==" saltValue="5cK2MkYC+bv1ZqeeRk5cUA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UrMWsEQcwthwhMB6wDO5VOb0MIraD92Wo3p1CHVBWDoqBIj2tLPhjVnmrJ/wJx3C2MqiyCPTrL+vvzhtBbFIfQ==" saltValue="/VLfWxpWvZ1fhpBUudX8KA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <customSheetViews>
     <customSheetView guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1573,9 +1564,12 @@
       <formula>$C$4="Your Name"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{66755ED4-3614-4EB7-8CFA-93192F3C08E4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1618,188 +1612,188 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="37"/>
-    <col min="7" max="7" width="14.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="37"/>
+    <col min="1" max="1" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="14.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="46" t="str">
+      <c r="A7" s="23" t="str">
         <f>'Percent Change'!A7</f>
         <v>Enter your</v>
       </c>
-      <c r="B7" s="46" t="str">
+      <c r="B7" s="23" t="str">
         <f>'Percent Change'!B7</f>
         <v>name in C4 and</v>
       </c>
-      <c r="C7" s="47" t="e">
+      <c r="C7" s="24" t="e">
         <f>B7-A7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D7" s="47" t="e">
+      <c r="D7" s="24" t="e">
         <f>C7/A7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E7" s="48" t="e">
+      <c r="E7" s="25" t="e">
         <f>D7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50" t="s">
+      <c r="F7" s="26"/>
+      <c r="G7" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="50"/>
+      <c r="H7" s="56"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A8" s="46" t="str">
+      <c r="A8" s="23" t="str">
         <f>'Percent Change'!A8</f>
         <v xml:space="preserve">your values </v>
       </c>
-      <c r="B8" s="46" t="str">
+      <c r="B8" s="23" t="str">
         <f>'Percent Change'!B8</f>
         <v>will appear</v>
       </c>
-      <c r="C8" s="47" t="e">
+      <c r="C8" s="24" t="e">
         <f>B8-A8</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D8" s="47" t="e">
+      <c r="D8" s="24" t="e">
         <f>C8/A8</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E8" s="48" t="e">
+      <c r="E8" s="25" t="e">
         <f>D8</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="52"/>
+      <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="G10" s="56" t="s">
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
+      <c r="G10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="28" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
-      <c r="G11" s="56" t="s">
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="G11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="57" t="s">
+      <c r="H11" s="28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
-      <c r="G12" s="56" t="s">
+      <c r="C12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="G12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="28" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="65" t="s">
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="66" t="s">
+      <c r="H14" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="64" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -1809,15 +1803,15 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="9">
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:E12"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:E12"/>
-    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="A7:B8">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Moved the sheet saying to ignore halo
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-1_Tech_Template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{16B44EE0-7408-4D79-8AF1-9BBCA345B6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{7AD382FE-BCEE-44BB-B434-7B306D2427A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="1470" windowWidth="20430" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Percent Change" sheetId="1" r:id="rId1"/>
-    <sheet name="Ignore Halo" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Random" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Random" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="ZZZ" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -874,6 +874,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -949,9 +952,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1195,13 +1195,21 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CAB9540D-B0CF-42A1-8201-F8F28DFDFC93}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B50912F6-D886-439A-8C2D-9AEE28C65B29}" diskRevisions="1" revisionId="1" version="2">
   <header guid="{CAB9540D-B0CF-42A1-8201-F8F28DFDFC93}" dateTime="2022-07-20T13:40:22" maxSheetId="5" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
       <sheetId val="3"/>
       <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B50912F6-D886-439A-8C2D-9AEE28C65B29}" dateTime="2022-07-20T14:37:11" maxSheetId="5" userName="Richard Ketchersid" r:id="rId2" minRId="1">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="2"/>
     </sheetIdMap>
   </header>
 </headers>
@@ -1211,9 +1219,18 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}" action="delete"/>
+  <rcv guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}" action="add"/>
+  <rsnm rId="1" sheetId="2" oldName="[QR_2-1_Tech_Template.xlsx]Ignore Halo" newName="[QR_2-1_Tech_Template.xlsx]ZZZ"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{CAB9540D-B0CF-42A1-8201-F8F28DFDFC93}" name="Richard Ketchersid" id="-1739522438" dateTime="2022-07-20T13:40:22"/>
+  <userInfo guid="{B50912F6-D886-439A-8C2D-9AEE28C65B29}" name="Richard Ketchersid" id="-1739578853" dateTime="2022-07-20T14:35:13"/>
 </users>
 </file>
 
@@ -1483,7 +1500,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1669,7 +1686,7 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <customSheetViews>
     <customSheetView guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C24" sqref="C24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1733,74 +1750,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5029BD-1F3F-4659-8ADE-18D051EA9DF2}">
-  <dimension ref="D7:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="7" spans="4:9">
-      <c r="D7" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-    </row>
-    <row r="8" spans="4:9" ht="15" customHeight="1">
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-    </row>
-    <row r="9" spans="4:9">
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-    </row>
-    <row r="10" spans="4:9">
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-    </row>
-    <row r="11" spans="4:9">
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-    </row>
-  </sheetData>
-  <customSheetViews>
-    <customSheetView guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}" state="hidden">
-      <selection activeCell="E19" sqref="E19"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-    </customSheetView>
-  </customSheetViews>
-  <mergeCells count="1">
-    <mergeCell ref="D7:I11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90B7FD0-59F4-4CAB-8656-0D8BCCB1BD32}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -1823,20 +1772,20 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="19" t="s">
         <v>46</v>
       </c>
@@ -1885,10 +1834,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="F7" s="25"/>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="59"/>
+      <c r="H7" s="60"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1">
       <c r="A8" s="22" t="str">
@@ -1913,17 +1862,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="61"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
       <c r="G10" s="26" t="s">
         <v>12</v>
       </c>
@@ -1932,9 +1881,9 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
       <c r="G11" s="26" t="s">
         <v>14</v>
       </c>
@@ -1943,9 +1892,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
       <c r="G12" s="26" t="s">
         <v>16</v>
       </c>
@@ -1962,11 +1911,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
       <c r="G14" s="28" t="s">
         <v>20</v>
       </c>
@@ -1976,22 +1925,22 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="30"/>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="53" t="s">
+      <c r="C15" s="72"/>
+      <c r="D15" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2028,7 +1977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E75AC65-D95A-4F82-A945-BA06112EA708}">
   <dimension ref="A1:W45"/>
   <sheetViews>
@@ -3563,7 +3512,84 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5029BD-1F3F-4659-8ADE-18D051EA9DF2}">
+  <dimension ref="D7:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7" spans="4:9">
+      <c r="D7" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="4:9" ht="15" customHeight="1">
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+    </row>
+    <row r="9" spans="4:9">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+    </row>
+    <row r="10" spans="4:9">
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+    </row>
+    <row r="11" spans="4:9">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{4BAD3247-7C98-43DD-8E27-2A61F2E9C82A}" state="hidden">
+      <selection activeCell="F25" sqref="F25"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
+  <mergeCells count="1">
+    <mergeCell ref="D7:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002FC4D7A32A34E94B953742578E0D227D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6062e902822a1ea35e0b6c93f60576e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d8c16f6f-632d-4fa9-9000-4a0cb55aa11b" xmlns:ns4="6588c10b-b5ed-4e95-9d69-08b9b2ce7055" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a7d56c96ea3c0bda530556fd5715147" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3803,15 +3829,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3822,6 +3839,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4248261A-3D09-4E75-A1C3-3D294EFE11B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DEFD836-FD30-4819-86F9-2317EB0EE1D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3841,14 +3866,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4248261A-3D09-4E75-A1C3-3D294EFE11B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{945F3AE1-9BD0-4BCF-A6FD-932ADCD78A39}">
   <ds:schemaRefs>

</xml_diff>